<commit_message>
dnd media works product codes
</commit_message>
<xml_diff>
--- a/dnd-media-works/checklist.xlsx
+++ b/dnd-media-works/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/dnd-media-works/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BD72F8-7C63-1749-94A1-210DEC160A08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE34B2DD-7477-9341-94E9-0BF5A41D07BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{183B78AA-1416-4B41-A4A5-2B582434C07C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{183B78AA-1416-4B41-A4A5-2B582434C07C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
   <si>
     <t>year</t>
   </si>
@@ -183,6 +183,45 @@
   </si>
   <si>
     <t>Dungeons &amp; Dragons Introductory Book &lt;&lt;Revised&gt;&gt;</t>
+  </si>
+  <si>
+    <t>product_code</t>
+  </si>
+  <si>
+    <t>5-1</t>
+  </si>
+  <si>
+    <t>1-1</t>
+  </si>
+  <si>
+    <t>1-3</t>
+  </si>
+  <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>1-4</t>
+  </si>
+  <si>
+    <t>1-6</t>
+  </si>
+  <si>
+    <t>1-9</t>
+  </si>
+  <si>
+    <t>1-5</t>
+  </si>
+  <si>
+    <t>1-7</t>
+  </si>
+  <si>
+    <t>1-8</t>
+  </si>
+  <si>
+    <t>1-10</t>
+  </si>
+  <si>
+    <t>1-11</t>
   </si>
 </sst>
 </file>
@@ -232,9 +271,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F75D5C8D-277A-9C44-B685-BC80EF2A91EC}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -563,7 +603,7 @@
     <col min="5" max="5" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -582,8 +622,11 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1994</v>
       </c>
@@ -602,8 +645,11 @@
       <c r="F2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1995</v>
       </c>
@@ -622,8 +668,11 @@
       <c r="F3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1996</v>
       </c>
@@ -642,8 +691,11 @@
       <c r="F4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1994</v>
       </c>
@@ -662,8 +714,11 @@
       <c r="F5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1994</v>
       </c>
@@ -682,8 +737,9 @@
       <c r="F6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1994</v>
       </c>
@@ -702,8 +758,11 @@
       <c r="F7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1994</v>
       </c>
@@ -722,8 +781,11 @@
       <c r="F8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1995</v>
       </c>
@@ -742,8 +804,11 @@
       <c r="F9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1995</v>
       </c>
@@ -762,8 +827,11 @@
       <c r="F10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1996</v>
       </c>
@@ -782,8 +850,11 @@
       <c r="F11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1996</v>
       </c>
@@ -802,8 +873,11 @@
       <c r="F12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1997</v>
       </c>
@@ -822,8 +896,11 @@
       <c r="F13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1993</v>
       </c>
@@ -841,6 +918,9 @@
       </c>
       <c r="F14" t="s">
         <v>22</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
product codes for fortune quest
</commit_message>
<xml_diff>
--- a/dnd-media-works/checklist.xlsx
+++ b/dnd-media-works/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/dnd-media-works/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE34B2DD-7477-9341-94E9-0BF5A41D07BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6482262-0199-684D-9A69-65E3A7DE250E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{183B78AA-1416-4B41-A4A5-2B582434C07C}"/>
   </bookViews>
@@ -188,40 +188,40 @@
     <t>product_code</t>
   </si>
   <si>
-    <t>5-1</t>
-  </si>
-  <si>
-    <t>1-1</t>
-  </si>
-  <si>
-    <t>1-3</t>
-  </si>
-  <si>
-    <t>1-2</t>
-  </si>
-  <si>
-    <t>1-4</t>
-  </si>
-  <si>
-    <t>1-6</t>
-  </si>
-  <si>
-    <t>1-9</t>
-  </si>
-  <si>
-    <t>1-5</t>
-  </si>
-  <si>
-    <t>1-7</t>
-  </si>
-  <si>
-    <t>1-8</t>
-  </si>
-  <si>
-    <t>1-10</t>
-  </si>
-  <si>
-    <t>1-11</t>
+    <t>G-1-9</t>
+  </si>
+  <si>
+    <t>G-1-4</t>
+  </si>
+  <si>
+    <t>G-1-6</t>
+  </si>
+  <si>
+    <t>G-1-2</t>
+  </si>
+  <si>
+    <t>G-1-3</t>
+  </si>
+  <si>
+    <t>G-1-1</t>
+  </si>
+  <si>
+    <t>G-1-5</t>
+  </si>
+  <si>
+    <t>G-1-7</t>
+  </si>
+  <si>
+    <t>G-1-8</t>
+  </si>
+  <si>
+    <t>G-1-10</t>
+  </si>
+  <si>
+    <t>G-1-11</t>
+  </si>
+  <si>
+    <t>G-5-1</t>
   </si>
 </sst>
 </file>
@@ -592,7 +592,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -646,7 +646,7 @@
         <v>19</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -669,7 +669,7 @@
         <v>19</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -692,7 +692,7 @@
         <v>19</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -759,7 +759,7 @@
         <v>20</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -782,7 +782,7 @@
         <v>20</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -805,7 +805,7 @@
         <v>22</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -828,7 +828,7 @@
         <v>22</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -851,7 +851,7 @@
         <v>22</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -874,7 +874,7 @@
         <v>22</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -897,7 +897,7 @@
         <v>22</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -920,7 +920,7 @@
         <v>22</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>